<commit_message>
rodapé editado e próximos jogos
</commit_message>
<xml_diff>
--- a/Tabela Premier League.xlsx
+++ b/Tabela Premier League.xlsx
@@ -18,12 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
   <si>
-    <t>5° Rod.</t>
-  </si>
-  <si>
-    <t>6° Rod.</t>
-  </si>
-  <si>
     <t>7° Rod.</t>
   </si>
   <si>
@@ -45,9 +39,6 @@
     <t>Sábado</t>
   </si>
   <si>
-    <t>Terça</t>
-  </si>
-  <si>
     <t>ARSENAL</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t xml:space="preserve">TOT (C) </t>
   </si>
   <si>
-    <t xml:space="preserve">C.PAL (C) </t>
-  </si>
-  <si>
     <t xml:space="preserve">BOU (C) </t>
   </si>
   <si>
@@ -231,9 +219,6 @@
     <t>BOU (F)</t>
   </si>
   <si>
-    <t>FUL (H)</t>
-  </si>
-  <si>
     <t>9° Rod.</t>
   </si>
   <si>
@@ -262,6 +247,21 @@
   </si>
   <si>
     <t>Nivel 1</t>
+  </si>
+  <si>
+    <t>10° Rod.</t>
+  </si>
+  <si>
+    <t>11° Rod.</t>
+  </si>
+  <si>
+    <t>Sexta</t>
+  </si>
+  <si>
+    <t>LIV ©</t>
+  </si>
+  <si>
+    <t>BHA (C)</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -447,11 +447,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -513,29 +524,41 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,22 +866,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="0.5703125" style="4" customWidth="1"/>
-    <col min="3" max="7" width="9.42578125" customWidth="1"/>
+    <col min="3" max="5" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="1" t="s">
@@ -868,520 +891,520 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="7">
-        <v>44803</v>
+        <v>44814</v>
       </c>
       <c r="D2" s="7">
-        <v>44807</v>
+        <v>44820</v>
       </c>
       <c r="E2" s="7">
-        <v>44814</v>
-      </c>
-      <c r="F2" s="7">
-        <v>44820</v>
-      </c>
-      <c r="G2" s="7">
         <v>44835</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F2" s="8">
+        <v>44842</v>
+      </c>
+      <c r="G2" s="8">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8">
-        <v>0.58333333333333337</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="D3" s="8">
-        <v>0.29166666666666669</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="E3" s="8">
         <v>0.29166666666666669</v>
       </c>
       <c r="F3" s="8">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="G3" s="8">
         <v>0.60416666666666663</v>
       </c>
-      <c r="G3" s="8">
-        <v>0.29166666666666669</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="30"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="23"/>
+      <c r="J5" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="L4" s="24"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="18" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>41</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="25"/>
-      <c r="L5" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>47</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>45</v>
+      <c r="F6" s="32" t="s">
+        <v>56</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="I6" s="24"/>
+      <c r="J6" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="19" t="s">
+      <c r="E7" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="28"/>
-      <c r="L7" s="30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I7" s="26"/>
+      <c r="J7" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="K8" s="27"/>
-      <c r="L8" s="30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="25"/>
+      <c r="J8" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>70</v>
+        <v>46</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="30" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>46</v>
+        <v>64</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>19</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="E15" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>61</v>
+        <v>38</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>66</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>63</v>
+        <v>44</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="6" t="s">
-        <v>42</v>
+      <c r="C17" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="18" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>69</v>
+        <v>34</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="20" t="s">
-        <v>52</v>
+      <c r="C19" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>36</v>
+        <v>64</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="20" t="s">
-        <v>51</v>
+      <c r="C20" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>62</v>
+        <v>37</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="20" t="s">
-        <v>44</v>
+      <c r="C21" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>56</v>
+      <c r="E22" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="20" t="s">
+      <c r="C23" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>63</v>
+        <v>44</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>35</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>47</v>
+      <c r="C24" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1434,7 +1457,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
bourne, brent, lei, liv, new
</commit_message>
<xml_diff>
--- a/Tabela Premier League.xlsx
+++ b/Tabela Premier League.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="80">
   <si>
     <t>Rodadas</t>
   </si>
@@ -141,9 +141,6 @@
     <t xml:space="preserve">WOL (C) </t>
   </si>
   <si>
-    <t xml:space="preserve">BHA (C) </t>
-  </si>
-  <si>
     <t xml:space="preserve">C.PA (C) </t>
   </si>
   <si>
@@ -207,15 +204,9 @@
     <t>BOU (F)</t>
   </si>
   <si>
-    <t>9° Rod.</t>
-  </si>
-  <si>
     <t>TOT (C)</t>
   </si>
   <si>
-    <t>C.PA (F)</t>
-  </si>
-  <si>
     <t>Dificuldade</t>
   </si>
   <si>
@@ -234,9 +225,6 @@
     <t>Nivel 1</t>
   </si>
   <si>
-    <t>10° Rod.</t>
-  </si>
-  <si>
     <t>11° Rod.</t>
   </si>
   <si>
@@ -262,6 +250,12 @@
   </si>
   <si>
     <t>ADIADO</t>
+  </si>
+  <si>
+    <t>15° Rod.</t>
+  </si>
+  <si>
+    <t>16° Rod.</t>
   </si>
 </sst>
 </file>
@@ -482,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -504,9 +498,6 @@
     <xf numFmtId="20" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -565,7 +556,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="6" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -574,31 +586,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="6" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -910,7 +898,7 @@
   <dimension ref="B2:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,17 +913,17 @@
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="29" t="s">
+      <c r="D2" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>78</v>
@@ -945,69 +933,69 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="7">
-        <v>44835</v>
+        <v>44848</v>
       </c>
       <c r="E3" s="7">
-        <v>44842</v>
+        <v>44852</v>
       </c>
       <c r="F3" s="7">
-        <v>44848</v>
+        <v>44856</v>
       </c>
       <c r="G3" s="7">
-        <v>44852</v>
+        <v>44863</v>
       </c>
       <c r="H3" s="7">
-        <v>44856</v>
+        <v>44870</v>
       </c>
       <c r="I3" s="7">
-        <v>44863</v>
+        <v>44877</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="8">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F4" s="8">
         <v>0.29166666666666669</v>
       </c>
-      <c r="E4" s="8">
+      <c r="G4" s="8">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H4" s="8">
         <v>0.39583333333333331</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="G4" s="8">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="H4" s="8">
-        <v>0.29166666666666669</v>
       </c>
       <c r="I4" s="8">
         <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>4</v>
@@ -1015,558 +1003,558 @@
       <c r="I5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" s="38"/>
+    </row>
+    <row r="6" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="22"/>
+      <c r="L6" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="23"/>
+      <c r="L7" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="25"/>
+      <c r="L8" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="L5" s="32"/>
-    </row>
-    <row r="6" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="19" t="s">
+    </row>
+    <row r="9" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="24"/>
+      <c r="L9" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="26"/>
+      <c r="L10" s="27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="H6" s="18" t="s">
+      <c r="I12" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="H21" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="19" t="s">
+      <c r="E25" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="24"/>
-      <c r="L7" s="28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="21" t="s">
+      <c r="F25" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="26"/>
-      <c r="L8" s="28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="25"/>
-      <c r="L9" s="28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="27"/>
-      <c r="L10" s="28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="19" t="s">
+      <c r="G25" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="38" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="I18" s="40" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I21" s="38" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="H23" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" s="37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="H25" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="I25" s="37" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="22"/>
+      <c r="B26" s="21"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="22"/>
+      <c r="B27" s="21"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="22"/>
+      <c r="B28" s="21"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="22"/>
+      <c r="B29" s="21"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="22"/>
+      <c r="B30" s="21"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="22"/>
+      <c r="B31" s="21"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="22"/>
+      <c r="B32" s="21"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="22"/>
+      <c r="B33" s="21"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="22"/>
+      <c r="B34" s="21"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="22"/>
+      <c r="B35" s="21"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="22"/>
+      <c r="B36" s="21"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="22"/>
+      <c r="B37" s="21"/>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="22"/>
+      <c r="B38" s="21"/>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="22"/>
+      <c r="B39" s="21"/>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="22"/>
+      <c r="B40" s="21"/>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="22"/>
+      <c r="B41" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>